<commit_message>
Updated the rubric for 2022. More suggestions for next year.
</commit_message>
<xml_diff>
--- a/TermProject/CS296N-TermProjectRubric.xlsx
+++ b/TermProject/CS296N-TermProjectRubric.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS296N-CourseMaterials/TermProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBACBE5-6264-534A-9E6F-44049B526056}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC503CF-BB7B-6847-B0A8-5A1515256498}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14380" xr2:uid="{A352453A-1606-7D43-A59A-E10A55784CED}"/>
+    <workbookView xWindow="13500" yWindow="780" windowWidth="12020" windowHeight="14380" activeTab="1" xr2:uid="{A352453A-1606-7D43-A59A-E10A55784CED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rubric" sheetId="1" r:id="rId1"/>
+    <sheet name="Scoring" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>Code Quality and Style</t>
   </si>
@@ -51,30 +52,15 @@
     <t>Authentication and authorization, 2 roles</t>
   </si>
   <si>
-    <t>Security testing</t>
-  </si>
-  <si>
-    <t>Load Testing</t>
-  </si>
-  <si>
     <t>Published to web</t>
   </si>
   <si>
     <t>Unit Tests</t>
   </si>
   <si>
-    <t>Documentation</t>
-  </si>
-  <si>
-    <t>Completed code review</t>
-  </si>
-  <si>
     <t>Interactive rich media</t>
   </si>
   <si>
-    <t>3 or more tables, 9 or more fields, 8 or more pages</t>
-  </si>
-  <si>
     <t>Navigation</t>
   </si>
   <si>
@@ -87,17 +73,23 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Best OO Design and coding practices</t>
-  </si>
-  <si>
     <t>Standard coding style</t>
+  </si>
+  <si>
+    <t>4 or more tables, 12 or more fields, 10 or more pages</t>
+  </si>
+  <si>
+    <t>Load testing</t>
+  </si>
+  <si>
+    <t>OO Design and coding practices (including Asyc)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -107,14 +99,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -142,10 +126,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,212 +444,375 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C2946B-FEFE-C947-8985-045316750FD9}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:G24"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="7.83203125" customWidth="1"/>
-    <col min="7" max="7" width="6.5" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" customWidth="1"/>
+    <col min="6" max="6" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>25</v>
+      </c>
+      <c r="F7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="E10">
+        <v>30</v>
+      </c>
+      <c r="F10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
+      <c r="E11">
+        <v>25</v>
+      </c>
+      <c r="F11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>50</v>
+      </c>
+      <c r="F12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13">
+        <v>50</v>
+      </c>
+      <c r="F13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>50</v>
+      </c>
+      <c r="F14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>30</v>
+      </c>
+      <c r="F15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="F18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21">
+        <f>SUM(E2:E19)</f>
+        <v>350</v>
+      </c>
+      <c r="F21">
+        <f>SUM(F2:F19)</f>
+        <v>350</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03468CBE-99B7-B64E-9ED0-C5235FA013E3}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="7.83203125" customWidth="1"/>
+    <col min="6" max="6" width="6.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="F6">
+      <c r="E4">
         <v>5</v>
       </c>
-      <c r="G6">
+      <c r="F4">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>25</v>
+      </c>
+      <c r="F7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10">
+        <v>30</v>
+      </c>
+      <c r="F10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>25</v>
+      </c>
+      <c r="F11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>50</v>
+      </c>
+      <c r="F12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13">
+        <v>50</v>
+      </c>
+      <c r="F13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>50</v>
+      </c>
+      <c r="F14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>30</v>
+      </c>
+      <c r="F15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="F18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>14</v>
       </c>
-      <c r="F9">
-        <v>25</v>
-      </c>
-      <c r="G9">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10">
-        <v>50</v>
-      </c>
-      <c r="G10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11">
-        <v>15</v>
-      </c>
-      <c r="G11">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12">
-        <v>30</v>
-      </c>
-      <c r="G12">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13">
-        <v>25</v>
-      </c>
-      <c r="G13">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14">
-        <v>50</v>
-      </c>
-      <c r="G14">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15">
-        <v>50</v>
-      </c>
-      <c r="G15">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17">
-        <v>50</v>
-      </c>
-      <c r="G17">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18">
-        <v>30</v>
-      </c>
-      <c r="G18">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>20</v>
+      <c r="E21">
+        <f>SUM(E2:E19)</f>
+        <v>350</v>
       </c>
       <c r="F21">
-        <v>10</v>
-      </c>
-      <c r="G21">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22">
-        <v>10</v>
-      </c>
-      <c r="G22">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24">
-        <f>SUM(F2:F22)</f>
-        <v>350</v>
-      </c>
-      <c r="G24">
-        <f>SUM(G2:G22)</f>
+        <f>SUM(F2:F19)</f>
         <v>350</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added an html version of the rubric
</commit_message>
<xml_diff>
--- a/TermProject/CS296N-TermProjectRubric.xlsx
+++ b/TermProject/CS296N-TermProjectRubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS296N-CourseMaterials/TermProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A9BEF0-205B-214D-AE2E-7CF5C77C08E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6B2FAD-5D02-2C4C-8F94-41633FFDC897}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36340" yWindow="2160" windowWidth="19300" windowHeight="18540" activeTab="1" xr2:uid="{A352453A-1606-7D43-A59A-E10A55784CED}"/>
+    <workbookView xWindow="-20040" yWindow="1840" windowWidth="19300" windowHeight="18540" xr2:uid="{A352453A-1606-7D43-A59A-E10A55784CED}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>Code Quality and Style</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>4+ model classes, 12+ fields, 10+ views, 8+ data views</t>
+  </si>
+  <si>
+    <t>Search (aka filtering)</t>
   </si>
 </sst>
 </file>
@@ -462,8 +465,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F21"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -473,7 +476,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -532,7 +535,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E11">
         <v>25</v>
@@ -610,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03468CBE-99B7-B64E-9ED0-C5235FA013E3}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E25" sqref="E25:F25"/>
     </sheetView>
   </sheetViews>

</xml_diff>